<commit_message>
Test Cases Automation updated
</commit_message>
<xml_diff>
--- a/Test Cases/Test Cases - Automation.xlsx
+++ b/Test Cases/Test Cases - Automation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bhase\eclipse-workspace\Capstone_Project_SauceDemo_Testing\Test Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E984CFE-AABC-4753-9C9A-B7F65CCFECF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{082011F2-19D1-42B1-996E-99CB44F9A8A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1298,8 +1298,8 @@
   </sheetPr>
   <dimension ref="A1:T40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>